<commit_message>
Hapus Edit Halaman Nilai
</commit_message>
<xml_diff>
--- a/excel upload.xlsx
+++ b/excel upload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\sistem_nilai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4F57C3-49A5-48FC-84AA-44CA07E0A457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35519BE5-9184-4153-98EE-18EBBD135BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{BB8F3E86-2CAE-4D25-BF2E-5967EC622955}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB8F3E86-2CAE-4D25-BF2E-5967EC622955}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,13 +444,13 @@
         <v>123</v>
       </c>
       <c r="C2">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="E2">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -461,13 +461,13 @@
         <v>124</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D3">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="E3">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -478,13 +478,13 @@
         <v>125</v>
       </c>
       <c r="C4">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4">
-        <v>11</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Menambah Semester & KKM
</commit_message>
<xml_diff>
--- a/excel upload.xlsx
+++ b/excel upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\sistem_nilai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35519BE5-9184-4153-98EE-18EBBD135BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C87D2E0-1C2A-438C-9031-272DE6A0A3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB8F3E86-2CAE-4D25-BF2E-5967EC622955}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,13 +444,13 @@
         <v>123</v>
       </c>
       <c r="C2">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="D2">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E2">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -461,13 +461,13 @@
         <v>124</v>
       </c>
       <c r="C3">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D3">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E3">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -478,13 +478,13 @@
         <v>125</v>
       </c>
       <c r="C4">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D4">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="E4">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>